<commit_message>
new LCA importing way
</commit_message>
<xml_diff>
--- a/exposan/bwaise/results/sysA_lca.xlsx
+++ b/exposan/bwaise/results/sysA_lca.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfca01abaf64aab7/Coding/es/exposan/bwaise/results/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_AF7EC3347248492913603333C62E517760B4E222" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0568FBE9-5FF6-6E4B-80FD-71BC66CD78B0}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="9980" yWindow="460" windowWidth="26020" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LCA" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -133,8 +139,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,8 +192,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -197,6 +206,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -243,7 +260,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -275,9 +292,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -309,6 +344,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -484,14 +537,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -511,46 +567,46 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C2">
-        <v>6473254.725</v>
+        <v>6473254.7249999996</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
-        <v>1812511.323</v>
+        <v>1812511.3230000001</v>
       </c>
       <c r="F2">
-        <v>0.05784384908321555</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1"/>
+        <v>5.7843849083215548E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
       <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C3">
-        <v>6473254.725</v>
+        <v>6473254.7249999996</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>1812511.323</v>
+        <v>1812511.3230000001</v>
       </c>
       <c r="F3">
-        <v>0.05784384908321555</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="1" t="s">
+        <v>5.7843849083215548E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -566,11 +622,11 @@
         <v>21577515.75</v>
       </c>
       <c r="F4">
-        <v>0.6886172509906613</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="1"/>
+        <v>0.68861725099066129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
@@ -584,11 +640,11 @@
         <v>21577515.75</v>
       </c>
       <c r="F5">
-        <v>0.6886172509906613</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="1" t="s">
+        <v>0.68861725099066129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -598,73 +654,73 @@
         <v>433.0444991846079</v>
       </c>
       <c r="D6">
-        <v>0.06671270848009403</v>
+        <v>6.671270848009403E-2</v>
       </c>
       <c r="E6">
         <v>129913.3497553824</v>
       </c>
       <c r="F6">
-        <v>0.004146008966557687</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1"/>
+        <v>4.1460089665576868E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
       <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C7">
-        <v>6058.139999999999</v>
+        <v>6058.1399999999994</v>
       </c>
       <c r="D7">
-        <v>0.933287291519906</v>
+        <v>0.93328729151990597</v>
       </c>
       <c r="E7">
         <v>1817442</v>
       </c>
       <c r="F7">
-        <v>0.05800120497536744</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1"/>
+        <v>5.800120497536744E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C8">
-        <v>6491.184499184607</v>
+        <v>6491.1844991846074</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8">
-        <v>1947355.349755382</v>
+        <v>1947355.3497553819</v>
       </c>
       <c r="F8">
-        <v>0.06214721394192513</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="1" t="s">
+        <v>6.2147213941925128E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C9">
-        <v>104348.4095</v>
+        <v>104348.40949999999</v>
       </c>
       <c r="D9">
-        <v>0.7308354553847088</v>
+        <v>0.73083545538470884</v>
       </c>
       <c r="E9">
-        <v>55304.65703500002</v>
+        <v>55304.657035000018</v>
       </c>
       <c r="F9">
-        <v>0.001764973379496805</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="1"/>
+        <v>1.7649733794968051E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
       <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
@@ -672,17 +728,17 @@
         <v>1451.211728244062</v>
       </c>
       <c r="D10">
-        <v>0.01016399760526182</v>
+        <v>1.0163997605261821E-2</v>
       </c>
       <c r="E10">
-        <v>769.1422159693531</v>
+        <v>769.14221596935306</v>
       </c>
       <c r="F10">
-        <v>2.454613425003207E-05</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="1"/>
+        <v>2.4546134250032069E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
       <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
@@ -690,17 +746,17 @@
         <v>13920</v>
       </c>
       <c r="D11">
-        <v>0.09749290466142797</v>
+        <v>9.7492904661427973E-2</v>
       </c>
       <c r="E11">
         <v>7377.6</v>
       </c>
       <c r="F11">
-        <v>0.0002354461324357371</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="1"/>
+        <v>2.354461324357371E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
       <c r="B12" s="1" t="s">
         <v>21</v>
       </c>
@@ -708,17 +764,17 @@
         <v>23060</v>
       </c>
       <c r="D12">
-        <v>0.1615076423486012</v>
+        <v>0.16150764234860121</v>
       </c>
       <c r="E12">
         <v>12221.8</v>
       </c>
       <c r="F12">
-        <v>0.0003900422280149495</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="1"/>
+        <v>3.9004222801494948E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
       <c r="B13" s="1" t="s">
         <v>17</v>
       </c>
@@ -729,14 +785,14 @@
         <v>1</v>
       </c>
       <c r="E13">
-        <v>75673.19925096938</v>
+        <v>75673.199250969381</v>
       </c>
       <c r="F13">
-        <v>0.002415007874197525</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="1" t="s">
+        <v>2.415007874197525E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -752,11 +808,11 @@
         <v>548000.4</v>
       </c>
       <c r="F14">
-        <v>0.01748869208865171</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="1"/>
+        <v>1.7488692088651711E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
       <c r="B15" s="1" t="s">
         <v>17</v>
       </c>
@@ -770,49 +826,49 @@
         <v>548000.4</v>
       </c>
       <c r="F15">
-        <v>0.01748869208865171</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="1" t="s">
+        <v>1.7488692088651711E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C16">
-        <v>287700.21</v>
+        <v>287700.21000000002</v>
       </c>
       <c r="D16">
-        <v>0.9473102251044178</v>
+        <v>0.94731022510441776</v>
       </c>
       <c r="E16">
-        <v>566769.4137</v>
+        <v>566769.41370000003</v>
       </c>
       <c r="F16">
-        <v>0.01808767979268804</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="1"/>
+        <v>1.8087679792688039E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
       <c r="B17" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C17">
-        <v>4539.973846153845</v>
+        <v>4539.9738461538454</v>
       </c>
       <c r="D17">
-        <v>0.01494876783777171</v>
+        <v>1.494876783777171E-2</v>
       </c>
       <c r="E17">
-        <v>8943.748476923076</v>
+        <v>8943.7484769230759</v>
       </c>
       <c r="F17">
-        <v>0.0002854276442704338</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="1"/>
+        <v>2.8542764427043381E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
       <c r="B18" s="1" t="s">
         <v>21</v>
       </c>
@@ -820,80 +876,80 @@
         <v>11462.02729411765</v>
       </c>
       <c r="D18">
-        <v>0.03774100705781051</v>
+        <v>3.7741007057810513E-2</v>
       </c>
       <c r="E18">
-        <v>22580.19376941176</v>
+        <v>22580.193769411759</v>
       </c>
       <c r="F18">
-        <v>0.0007206163647605627</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="1"/>
+        <v>7.2061636476056267E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="2"/>
       <c r="B19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C19">
-        <v>303702.2111402715</v>
+        <v>303702.21114027151</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19">
-        <v>598293.3559463349</v>
+        <v>598293.35594633489</v>
       </c>
       <c r="F19">
-        <v>0.01909372380171903</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="1" t="s">
+        <v>1.9093723801719031E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C20">
-        <v>90545649.425</v>
+        <v>90545649.424999997</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20">
-        <v>1086547.7931</v>
+        <v>1086547.7930999999</v>
       </c>
       <c r="F20">
-        <v>0.03467570423877418</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="1"/>
+        <v>3.4675704238774183E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="2"/>
       <c r="B21" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C21">
-        <v>90545649.425</v>
+        <v>90545649.424999997</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21">
-        <v>1086547.7931</v>
+        <v>1086547.7930999999</v>
       </c>
       <c r="F21">
-        <v>0.03467570423877418</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="1" t="s">
+        <v>3.4675704238774183E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C22">
-        <v>958287.1578125</v>
+        <v>958287.15781250002</v>
       </c>
       <c r="D22">
         <v>0.9325618456531295</v>
@@ -902,29 +958,29 @@
         <v>2443632.252421875</v>
       </c>
       <c r="F22">
-        <v>0.07798522052265768</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="1"/>
+        <v>7.7985220522657675E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="2"/>
       <c r="B23" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C23">
-        <v>69298.47876407848</v>
+        <v>69298.478764078478</v>
       </c>
       <c r="D23">
-        <v>0.0674381543468705</v>
+        <v>6.7438154346870505E-2</v>
       </c>
       <c r="E23">
-        <v>176711.1208484001</v>
+        <v>176711.12084840011</v>
       </c>
       <c r="F23">
-        <v>0.005639496579123286</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="1"/>
+        <v>5.6394965791232857E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="2"/>
       <c r="B24" s="1" t="s">
         <v>17</v>
       </c>
@@ -935,51 +991,51 @@
         <v>1</v>
       </c>
       <c r="E24">
-        <v>2620343.373270275</v>
+        <v>2620343.3732702751</v>
       </c>
       <c r="F24">
-        <v>0.08362471710178096</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="1" t="s">
+        <v>8.362471710178096E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C25">
-        <v>5422.920625</v>
+        <v>5422.9206249999997</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25">
-        <v>1068315.363125</v>
+        <v>1068315.3631249999</v>
       </c>
       <c r="F25">
-        <v>0.03409384087907467</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="1"/>
+        <v>3.4093840879074667E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="2"/>
       <c r="B26" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C26">
-        <v>5422.920625</v>
+        <v>5422.9206249999997</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26">
-        <v>1068315.363125</v>
+        <v>1068315.3631249999</v>
       </c>
       <c r="F26">
-        <v>0.03409384087907467</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>3.4093840879074667E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>15</v>
       </c>
@@ -993,7 +1049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>23</v>
       </c>
@@ -1013,45 +1069,45 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C31">
-        <v>4932003.600000003</v>
+        <v>4932003.6000000034</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31">
-        <v>956808.6984000007</v>
+        <v>956808.69840000069</v>
       </c>
       <c r="F31">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="1"/>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="2"/>
       <c r="B32" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C32">
-        <v>4932003.600000003</v>
+        <v>4932003.6000000034</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32">
-        <v>956808.6984000007</v>
+        <v>956808.69840000069</v>
       </c>
       <c r="F32">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>15</v>
       </c>
@@ -1059,13 +1115,13 @@
         <v>22</v>
       </c>
       <c r="E33">
-        <v>956808.6984000007</v>
+        <v>956808.69840000069</v>
       </c>
       <c r="F33">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>27</v>
       </c>
@@ -1079,35 +1135,35 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B37">
-        <v>4911764.802095694</v>
+        <v>4911764.8020956935</v>
       </c>
       <c r="C37">
-        <v>137529414.4586794</v>
+        <v>137529414.45867941</v>
       </c>
       <c r="D37">
-        <v>1.206118572181886</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+        <v>1.2061185721818859</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B38">
-        <v>2982.083297928012</v>
+        <v>2982.0832979280121</v>
       </c>
       <c r="C38">
-        <v>790252.0739509232</v>
+        <v>790252.07395092316</v>
       </c>
       <c r="D38">
-        <v>0.006930427987707539</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+        <v>6.9304279877075393E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>30</v>
       </c>
@@ -1115,13 +1171,13 @@
         <v>1979814.487023849</v>
       </c>
       <c r="C39">
-        <v>-2969721.730535773</v>
+        <v>-2969721.7305357731</v>
       </c>
       <c r="D39">
-        <v>-0.02604414879180254</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+        <v>-2.604414879180254E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>31</v>
       </c>
@@ -1132,52 +1188,52 @@
         <v>-17438111.03414942</v>
       </c>
       <c r="D40">
-        <v>-0.1529304088499313</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
+        <v>-0.15293040884993131</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B41">
-        <v>345811.850976271</v>
+        <v>345811.85097627097</v>
       </c>
       <c r="C41">
-        <v>-1694478.069783728</v>
+        <v>-1694478.0697837281</v>
       </c>
       <c r="D41">
-        <v>-0.01486039534280944</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
+        <v>-1.4860395342809441E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B42">
-        <v>301871.7843221913</v>
+        <v>301871.78432219132</v>
       </c>
       <c r="C42">
-        <v>-452807.676483287</v>
+        <v>-452807.67648328701</v>
       </c>
       <c r="D42">
-        <v>-0.003971075935883569</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+        <v>-3.9710759358835687E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B43">
-        <v>127963.099855838</v>
+        <v>127963.09985583799</v>
       </c>
       <c r="C43">
-        <v>-691000.7392215254</v>
+        <v>-691000.73922152538</v>
       </c>
       <c r="D43">
-        <v>-0.006060004168903788</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+        <v>-6.0600041689037876E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>35</v>
       </c>
@@ -1188,10 +1244,10 @@
         <v>-1047101.101558584</v>
       </c>
       <c r="D44">
-        <v>-0.009182967080263151</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>-9.1829670802631505E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>15</v>
       </c>
@@ -1202,7 +1258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>36</v>
       </c>
@@ -1216,7 +1272,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>37</v>
       </c>
@@ -1230,7 +1286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>15</v>
       </c>
@@ -1243,16 +1299,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A31:A32"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A13"/>
     <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A31:A32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update with new biosteam
</commit_message>
<xml_diff>
--- a/exposan/bwaise/results/sysA_lca.xlsx
+++ b/exposan/bwaise/results/sysA_lca.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10314"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfca01abaf64aab7/Coding/es/exposan/bwaise/results/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_AF7EC3347248492913603333C62E517760B4E222" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0568FBE9-5FF6-6E4B-80FD-71BC66CD78B0}"/>
   <bookViews>
-    <workbookView xWindow="9980" yWindow="460" windowWidth="26020" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="LCA" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -94,7 +88,7 @@
     <t>Transportation</t>
   </si>
   <si>
-    <t>Trucking [tonne*km]</t>
+    <t>item26 [tonne*km]</t>
   </si>
   <si>
     <t>A3</t>
@@ -133,14 +127,14 @@
     <t>Other</t>
   </si>
   <si>
-    <t>e_item [kWh]</t>
+    <t>E_item [kWh]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,11 +186,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -206,14 +197,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -260,7 +243,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -292,27 +275,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -344,24 +309,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -537,17 +484,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -567,46 +511,46 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C2">
-        <v>6473254.7249999996</v>
+        <v>6473254.725</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
-        <v>1812511.3230000001</v>
+        <v>1812511.323</v>
       </c>
       <c r="F2">
-        <v>5.7843849083215548E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
+        <v>0.05784384908321555</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C3">
-        <v>6473254.7249999996</v>
+        <v>6473254.725</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>1812511.3230000001</v>
+        <v>1812511.323</v>
       </c>
       <c r="F3">
-        <v>5.7843849083215548E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+        <v>0.05784384908321555</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -622,11 +566,11 @@
         <v>21577515.75</v>
       </c>
       <c r="F4">
-        <v>0.68861725099066129</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
+        <v>0.6886172509906613</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
@@ -640,11 +584,11 @@
         <v>21577515.75</v>
       </c>
       <c r="F5">
-        <v>0.68861725099066129</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+        <v>0.6886172509906613</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -654,73 +598,73 @@
         <v>433.0444991846079</v>
       </c>
       <c r="D6">
-        <v>6.671270848009403E-2</v>
+        <v>0.06671270848009403</v>
       </c>
       <c r="E6">
         <v>129913.3497553824</v>
       </c>
       <c r="F6">
-        <v>4.1460089665576868E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
+        <v>0.004146008966557687</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C7">
-        <v>6058.1399999999994</v>
+        <v>6058.139999999999</v>
       </c>
       <c r="D7">
-        <v>0.93328729151990597</v>
+        <v>0.933287291519906</v>
       </c>
       <c r="E7">
         <v>1817442</v>
       </c>
       <c r="F7">
-        <v>5.800120497536744E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
+        <v>0.05800120497536744</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C8">
-        <v>6491.1844991846074</v>
+        <v>6491.184499184607</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8">
-        <v>1947355.3497553819</v>
+        <v>1947355.349755382</v>
       </c>
       <c r="F8">
-        <v>6.2147213941925128E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+        <v>0.06214721394192513</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C9">
-        <v>104348.40949999999</v>
+        <v>104348.4095</v>
       </c>
       <c r="D9">
-        <v>0.73083545538470884</v>
+        <v>0.7308354553847088</v>
       </c>
       <c r="E9">
-        <v>55304.657035000018</v>
+        <v>55304.65703500002</v>
       </c>
       <c r="F9">
-        <v>1.7649733794968051E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
+        <v>0.001764973379496805</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
@@ -728,17 +672,17 @@
         <v>1451.211728244062</v>
       </c>
       <c r="D10">
-        <v>1.0163997605261821E-2</v>
+        <v>0.01016399760526182</v>
       </c>
       <c r="E10">
-        <v>769.14221596935306</v>
+        <v>769.1422159693531</v>
       </c>
       <c r="F10">
-        <v>2.4546134250032069E-5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
+        <v>2.454613425003207E-05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
@@ -746,17 +690,17 @@
         <v>13920</v>
       </c>
       <c r="D11">
-        <v>9.7492904661427973E-2</v>
+        <v>0.09749290466142797</v>
       </c>
       <c r="E11">
         <v>7377.6</v>
       </c>
       <c r="F11">
-        <v>2.354461324357371E-4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
+        <v>0.0002354461324357371</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>21</v>
       </c>
@@ -764,17 +708,17 @@
         <v>23060</v>
       </c>
       <c r="D12">
-        <v>0.16150764234860121</v>
+        <v>0.1615076423486012</v>
       </c>
       <c r="E12">
         <v>12221.8</v>
       </c>
       <c r="F12">
-        <v>3.9004222801494948E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
+        <v>0.0003900422280149495</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>17</v>
       </c>
@@ -785,14 +729,14 @@
         <v>1</v>
       </c>
       <c r="E13">
-        <v>75673.199250969381</v>
+        <v>75673.19925096938</v>
       </c>
       <c r="F13">
-        <v>2.415007874197525E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+        <v>0.002415007874197525</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -808,11 +752,11 @@
         <v>548000.4</v>
       </c>
       <c r="F14">
-        <v>1.7488692088651711E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
+        <v>0.01748869208865171</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
         <v>17</v>
       </c>
@@ -826,49 +770,49 @@
         <v>548000.4</v>
       </c>
       <c r="F15">
-        <v>1.7488692088651711E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+        <v>0.01748869208865171</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C16">
-        <v>287700.21000000002</v>
+        <v>287700.21</v>
       </c>
       <c r="D16">
-        <v>0.94731022510441776</v>
+        <v>0.9473102251044178</v>
       </c>
       <c r="E16">
-        <v>566769.41370000003</v>
+        <v>566769.4137</v>
       </c>
       <c r="F16">
-        <v>1.8087679792688039E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
+        <v>0.01808767979268804</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C17">
-        <v>4539.9738461538454</v>
+        <v>4539.973846153845</v>
       </c>
       <c r="D17">
-        <v>1.494876783777171E-2</v>
+        <v>0.01494876783777171</v>
       </c>
       <c r="E17">
-        <v>8943.7484769230759</v>
+        <v>8943.748476923076</v>
       </c>
       <c r="F17">
-        <v>2.8542764427043381E-4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
+        <v>0.0002854276442704338</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
         <v>21</v>
       </c>
@@ -876,80 +820,80 @@
         <v>11462.02729411765</v>
       </c>
       <c r="D18">
-        <v>3.7741007057810513E-2</v>
+        <v>0.03774100705781051</v>
       </c>
       <c r="E18">
-        <v>22580.193769411759</v>
+        <v>22580.19376941176</v>
       </c>
       <c r="F18">
-        <v>7.2061636476056267E-4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
+        <v>0.0007206163647605627</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C19">
-        <v>303702.21114027151</v>
+        <v>303702.2111402715</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19">
-        <v>598293.35594633489</v>
+        <v>598293.3559463349</v>
       </c>
       <c r="F19">
-        <v>1.9093723801719031E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+        <v>0.01909372380171903</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C20">
-        <v>90545649.424999997</v>
+        <v>90545649.425</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20">
-        <v>1086547.7930999999</v>
+        <v>1086547.7931</v>
       </c>
       <c r="F20">
-        <v>3.4675704238774183E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
+        <v>0.03467570423877418</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C21">
-        <v>90545649.424999997</v>
+        <v>90545649.425</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21">
-        <v>1086547.7930999999</v>
+        <v>1086547.7931</v>
       </c>
       <c r="F21">
-        <v>3.4675704238774183E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+        <v>0.03467570423877418</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C22">
-        <v>958287.15781250002</v>
+        <v>958287.1578125</v>
       </c>
       <c r="D22">
         <v>0.9325618456531295</v>
@@ -958,29 +902,29 @@
         <v>2443632.252421875</v>
       </c>
       <c r="F22">
-        <v>7.7985220522657675E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
+        <v>0.07798522052265768</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C23">
-        <v>69298.478764078478</v>
+        <v>69298.47876407848</v>
       </c>
       <c r="D23">
-        <v>6.7438154346870505E-2</v>
+        <v>0.0674381543468705</v>
       </c>
       <c r="E23">
-        <v>176711.12084840011</v>
+        <v>176711.1208484001</v>
       </c>
       <c r="F23">
-        <v>5.6394965791232857E-3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="2"/>
+        <v>0.005639496579123286</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
         <v>17</v>
       </c>
@@ -991,51 +935,51 @@
         <v>1</v>
       </c>
       <c r="E24">
-        <v>2620343.3732702751</v>
+        <v>2620343.373270275</v>
       </c>
       <c r="F24">
-        <v>8.362471710178096E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+        <v>0.08362471710178096</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C25">
-        <v>5422.9206249999997</v>
+        <v>5422.920625</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25">
-        <v>1068315.3631249999</v>
+        <v>1068315.363125</v>
       </c>
       <c r="F25">
-        <v>3.4093840879074667E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="2"/>
+        <v>0.03409384087907467</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C26">
-        <v>5422.9206249999997</v>
+        <v>5422.920625</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26">
-        <v>1068315.3631249999</v>
+        <v>1068315.363125</v>
       </c>
       <c r="F26">
-        <v>3.4093840879074667E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.03409384087907467</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
         <v>15</v>
       </c>
@@ -1049,7 +993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
         <v>23</v>
       </c>
@@ -1069,45 +1013,45 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+    <row r="31" spans="1:6">
+      <c r="A31" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C31">
-        <v>4932003.6000000034</v>
+        <v>4932003.600000003</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31">
-        <v>956808.69840000069</v>
+        <v>956808.6984000007</v>
       </c>
       <c r="F31">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="2"/>
+    <row r="32" spans="1:6">
+      <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C32">
-        <v>4932003.6000000034</v>
+        <v>4932003.600000003</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32">
-        <v>956808.69840000069</v>
+        <v>956808.6984000007</v>
       </c>
       <c r="F32">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6">
       <c r="A33" s="1" t="s">
         <v>15</v>
       </c>
@@ -1115,13 +1059,13 @@
         <v>22</v>
       </c>
       <c r="E33">
-        <v>956808.69840000069</v>
+        <v>956808.6984000007</v>
       </c>
       <c r="F33">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6">
       <c r="A36" s="1" t="s">
         <v>27</v>
       </c>
@@ -1135,35 +1079,35 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6">
       <c r="A37" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B37">
-        <v>4911764.8020956935</v>
+        <v>4911701.166447819</v>
       </c>
       <c r="C37">
-        <v>137529414.45867941</v>
+        <v>137527632.6605389</v>
       </c>
       <c r="D37">
-        <v>1.2061185721818859</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1.206121793078792</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B38">
-        <v>2982.0832979280121</v>
+        <v>2982.083297928013</v>
       </c>
       <c r="C38">
-        <v>790252.07395092316</v>
+        <v>790252.0739509233</v>
       </c>
       <c r="D38">
-        <v>6.9304279877075393E-3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.006930536285537385</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" s="1" t="s">
         <v>30</v>
       </c>
@@ -1171,13 +1115,13 @@
         <v>1979814.487023849</v>
       </c>
       <c r="C39">
-        <v>-2969721.7305357731</v>
+        <v>-2969721.730535773</v>
       </c>
       <c r="D39">
-        <v>-2.604414879180254E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-0.026044555768803</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" s="1" t="s">
         <v>31</v>
       </c>
@@ -1185,80 +1129,80 @@
         <v>3229279.821138782</v>
       </c>
       <c r="C40">
-        <v>-17438111.03414942</v>
+        <v>-17438111.03414943</v>
       </c>
       <c r="D40">
-        <v>-0.15293040884993131</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-0.1529327986058634</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B41">
-        <v>345811.85097627097</v>
+        <v>345811.8509762709</v>
       </c>
       <c r="C41">
-        <v>-1694478.0697837281</v>
+        <v>-1694478.069783727</v>
       </c>
       <c r="D41">
-        <v>-1.4860395342809441E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-0.01486062755769848</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B42">
-        <v>301871.78432219132</v>
+        <v>301871.7843221913</v>
       </c>
       <c r="C42">
-        <v>-452807.67648328701</v>
+        <v>-452807.676483287</v>
       </c>
       <c r="D42">
-        <v>-3.9710759358835687E-3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-0.003971137989613406</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B43">
-        <v>127963.09985583799</v>
+        <v>127963.0998558381</v>
       </c>
       <c r="C43">
-        <v>-691000.73922152538</v>
+        <v>-691000.7392215255</v>
       </c>
       <c r="D43">
-        <v>-6.0600041689037876E-3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-0.006060098865119015</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B44">
-        <v>213694.1023588948</v>
+        <v>213694.1023588947</v>
       </c>
       <c r="C44">
         <v>-1047101.101558584</v>
       </c>
       <c r="D44">
-        <v>-9.1829670802631505E-3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-0.009183110577231602</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C45">
-        <v>114026446.180898</v>
+        <v>114024664.3827575</v>
       </c>
       <c r="D45">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6">
       <c r="A48" s="1" t="s">
         <v>36</v>
       </c>
@@ -1272,7 +1216,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4">
       <c r="A49" s="1" t="s">
         <v>37</v>
       </c>
@@ -1286,7 +1230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4">
       <c r="A50" s="1" t="s">
         <v>15</v>
       </c>
@@ -1299,16 +1243,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A13"/>
+    <mergeCell ref="A14:A15"/>
     <mergeCell ref="A16:A19"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="A22:A24"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A9:A13"/>
-    <mergeCell ref="A14:A15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update results (all minor with most being formatting changes
</commit_message>
<xml_diff>
--- a/exposan/bwaise/results/sysA_lca.xlsx
+++ b/exposan/bwaise/results/sysA_lca.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfca01abaf64aab7/Coding/es/exposan/bwaise/results/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_AF7EC334C04848CC09694F1B952C58BD60B4E223" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{308E5445-4921-9A4A-AD00-B9F817516E7B}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="23380" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LCA" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -133,8 +139,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,8 +192,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -197,6 +206,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -243,7 +260,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -275,9 +292,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -309,6 +344,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -484,14 +537,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -511,46 +567,46 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C2">
-        <v>6473254.725</v>
+        <v>6473254.7249999996</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
-        <v>1812511.323</v>
+        <v>1812511.3230000001</v>
       </c>
       <c r="F2">
-        <v>0.05784384908321555</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1"/>
+        <v>5.7843849083215548E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
       <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C3">
-        <v>6473254.725</v>
+        <v>6473254.7249999996</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>1812511.323</v>
+        <v>1812511.3230000001</v>
       </c>
       <c r="F3">
-        <v>0.05784384908321555</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="1" t="s">
+        <v>5.7843849083215548E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -566,11 +622,11 @@
         <v>21577515.75</v>
       </c>
       <c r="F4">
-        <v>0.6886172509906613</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="1"/>
+        <v>0.68861725099066129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
@@ -584,11 +640,11 @@
         <v>21577515.75</v>
       </c>
       <c r="F5">
-        <v>0.6886172509906613</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="1" t="s">
+        <v>0.68861725099066129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -598,73 +654,73 @@
         <v>433.0444991846079</v>
       </c>
       <c r="D6">
-        <v>0.06671270848009403</v>
+        <v>6.671270848009403E-2</v>
       </c>
       <c r="E6">
         <v>129913.3497553824</v>
       </c>
       <c r="F6">
-        <v>0.004146008966557687</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1"/>
+        <v>4.1460089665576868E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
       <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C7">
-        <v>6058.139999999999</v>
+        <v>6058.1399999999994</v>
       </c>
       <c r="D7">
-        <v>0.933287291519906</v>
+        <v>0.93328729151990597</v>
       </c>
       <c r="E7">
         <v>1817442</v>
       </c>
       <c r="F7">
-        <v>0.05800120497536744</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1"/>
+        <v>5.800120497536744E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C8">
-        <v>6491.184499184607</v>
+        <v>6491.1844991846074</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8">
-        <v>1947355.349755382</v>
+        <v>1947355.3497553819</v>
       </c>
       <c r="F8">
-        <v>0.06214721394192513</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="1" t="s">
+        <v>6.2147213941925128E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C9">
-        <v>104348.4095</v>
+        <v>104348.40949999999</v>
       </c>
       <c r="D9">
-        <v>0.7308354553847088</v>
+        <v>0.73083545538470884</v>
       </c>
       <c r="E9">
-        <v>55304.65703500002</v>
+        <v>55304.657035000018</v>
       </c>
       <c r="F9">
-        <v>0.001764973379496805</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="1"/>
+        <v>1.7649733794968051E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
       <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
@@ -672,17 +728,17 @@
         <v>1451.211728244062</v>
       </c>
       <c r="D10">
-        <v>0.01016399760526182</v>
+        <v>1.0163997605261821E-2</v>
       </c>
       <c r="E10">
-        <v>769.1422159693531</v>
+        <v>769.14221596935306</v>
       </c>
       <c r="F10">
-        <v>2.454613425003207E-05</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="1"/>
+        <v>2.4546134250032069E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
       <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
@@ -690,17 +746,17 @@
         <v>13920</v>
       </c>
       <c r="D11">
-        <v>0.09749290466142797</v>
+        <v>9.7492904661427973E-2</v>
       </c>
       <c r="E11">
         <v>7377.6</v>
       </c>
       <c r="F11">
-        <v>0.0002354461324357371</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="1"/>
+        <v>2.354461324357371E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
       <c r="B12" s="1" t="s">
         <v>21</v>
       </c>
@@ -708,17 +764,17 @@
         <v>23060</v>
       </c>
       <c r="D12">
-        <v>0.1615076423486012</v>
+        <v>0.16150764234860121</v>
       </c>
       <c r="E12">
         <v>12221.8</v>
       </c>
       <c r="F12">
-        <v>0.0003900422280149495</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="1"/>
+        <v>3.9004222801494948E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
       <c r="B13" s="1" t="s">
         <v>17</v>
       </c>
@@ -729,14 +785,14 @@
         <v>1</v>
       </c>
       <c r="E13">
-        <v>75673.19925096938</v>
+        <v>75673.199250969381</v>
       </c>
       <c r="F13">
-        <v>0.002415007874197525</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="1" t="s">
+        <v>2.415007874197525E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -752,11 +808,11 @@
         <v>548000.4</v>
       </c>
       <c r="F14">
-        <v>0.01748869208865171</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="1"/>
+        <v>1.7488692088651711E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
       <c r="B15" s="1" t="s">
         <v>17</v>
       </c>
@@ -770,49 +826,49 @@
         <v>548000.4</v>
       </c>
       <c r="F15">
-        <v>0.01748869208865171</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="1" t="s">
+        <v>1.7488692088651711E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C16">
-        <v>287700.21</v>
+        <v>287700.21000000002</v>
       </c>
       <c r="D16">
-        <v>0.9473102251044178</v>
+        <v>0.94731022510441776</v>
       </c>
       <c r="E16">
-        <v>566769.4137</v>
+        <v>566769.41370000003</v>
       </c>
       <c r="F16">
-        <v>0.01808767979268804</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="1"/>
+        <v>1.8087679792688039E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
       <c r="B17" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C17">
-        <v>4539.973846153845</v>
+        <v>4539.9738461538454</v>
       </c>
       <c r="D17">
-        <v>0.01494876783777171</v>
+        <v>1.494876783777171E-2</v>
       </c>
       <c r="E17">
-        <v>8943.748476923076</v>
+        <v>8943.7484769230759</v>
       </c>
       <c r="F17">
-        <v>0.0002854276442704338</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="1"/>
+        <v>2.8542764427043381E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
       <c r="B18" s="1" t="s">
         <v>21</v>
       </c>
@@ -820,80 +876,80 @@
         <v>11462.02729411765</v>
       </c>
       <c r="D18">
-        <v>0.03774100705781051</v>
+        <v>3.7741007057810513E-2</v>
       </c>
       <c r="E18">
-        <v>22580.19376941176</v>
+        <v>22580.193769411759</v>
       </c>
       <c r="F18">
-        <v>0.0007206163647605627</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="1"/>
+        <v>7.2061636476056267E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="2"/>
       <c r="B19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C19">
-        <v>303702.2111402715</v>
+        <v>303702.21114027151</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19">
-        <v>598293.3559463349</v>
+        <v>598293.35594633489</v>
       </c>
       <c r="F19">
-        <v>0.01909372380171903</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="1" t="s">
+        <v>1.9093723801719031E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C20">
-        <v>90545649.425</v>
+        <v>90545649.424999997</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20">
-        <v>1086547.7931</v>
+        <v>1086547.7930999999</v>
       </c>
       <c r="F20">
-        <v>0.03467570423877418</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="1"/>
+        <v>3.4675704238774183E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="2"/>
       <c r="B21" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C21">
-        <v>90545649.425</v>
+        <v>90545649.424999997</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21">
-        <v>1086547.7931</v>
+        <v>1086547.7930999999</v>
       </c>
       <c r="F21">
-        <v>0.03467570423877418</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="1" t="s">
+        <v>3.4675704238774183E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C22">
-        <v>958287.1578125</v>
+        <v>958287.15781250002</v>
       </c>
       <c r="D22">
         <v>0.9325618456531295</v>
@@ -902,29 +958,29 @@
         <v>2443632.252421875</v>
       </c>
       <c r="F22">
-        <v>0.07798522052265768</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="1"/>
+        <v>7.7985220522657675E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="2"/>
       <c r="B23" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C23">
-        <v>69298.47876407848</v>
+        <v>69298.478764078478</v>
       </c>
       <c r="D23">
-        <v>0.0674381543468705</v>
+        <v>6.7438154346870505E-2</v>
       </c>
       <c r="E23">
-        <v>176711.1208484001</v>
+        <v>176711.12084840011</v>
       </c>
       <c r="F23">
-        <v>0.005639496579123286</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="1"/>
+        <v>5.6394965791232857E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="2"/>
       <c r="B24" s="1" t="s">
         <v>17</v>
       </c>
@@ -935,51 +991,51 @@
         <v>1</v>
       </c>
       <c r="E24">
-        <v>2620343.373270275</v>
+        <v>2620343.3732702751</v>
       </c>
       <c r="F24">
-        <v>0.08362471710178096</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="1" t="s">
+        <v>8.362471710178096E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C25">
-        <v>5422.920625</v>
+        <v>5422.9206249999997</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25">
-        <v>1068315.363125</v>
+        <v>1068315.3631249999</v>
       </c>
       <c r="F25">
-        <v>0.03409384087907467</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="1"/>
+        <v>3.4093840879074667E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="2"/>
       <c r="B26" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C26">
-        <v>5422.920625</v>
+        <v>5422.9206249999997</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26">
-        <v>1068315.363125</v>
+        <v>1068315.3631249999</v>
       </c>
       <c r="F26">
-        <v>0.03409384087907467</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>3.4093840879074667E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>15</v>
       </c>
@@ -993,7 +1049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>23</v>
       </c>
@@ -1013,45 +1069,45 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C31">
-        <v>4932003.600000003</v>
+        <v>4932003.6000000034</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31">
-        <v>956808.6984000007</v>
+        <v>956808.69840000069</v>
       </c>
       <c r="F31">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="1"/>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="2"/>
       <c r="B32" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C32">
-        <v>4932003.600000003</v>
+        <v>4932003.6000000034</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32">
-        <v>956808.6984000007</v>
+        <v>956808.69840000069</v>
       </c>
       <c r="F32">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>15</v>
       </c>
@@ -1059,13 +1115,13 @@
         <v>22</v>
       </c>
       <c r="E33">
-        <v>956808.6984000007</v>
+        <v>956808.69840000069</v>
       </c>
       <c r="F33">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>27</v>
       </c>
@@ -1079,35 +1135,35 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B37">
-        <v>4911701.166447819</v>
+        <v>4911701.1664478192</v>
       </c>
       <c r="C37">
-        <v>137527632.6605389</v>
+        <v>137527632.66053891</v>
       </c>
       <c r="D37">
         <v>1.206121793078792</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B38">
-        <v>2982.083297928013</v>
+        <v>2982.0832979280131</v>
       </c>
       <c r="C38">
-        <v>790252.0739509233</v>
+        <v>790252.07395092328</v>
       </c>
       <c r="D38">
-        <v>0.006930536285537385</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+        <v>6.9305362855373847E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>30</v>
       </c>
@@ -1115,13 +1171,13 @@
         <v>1979814.487023849</v>
       </c>
       <c r="C39">
-        <v>-2969721.730535773</v>
+        <v>-2969721.7305357731</v>
       </c>
       <c r="D39">
-        <v>-0.026044555768803</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+        <v>-2.6044555768803001E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>31</v>
       </c>
@@ -1129,41 +1185,41 @@
         <v>3229279.821138782</v>
       </c>
       <c r="C40">
-        <v>-17438111.03414943</v>
+        <v>-17438111.034149431</v>
       </c>
       <c r="D40">
         <v>-0.1529327986058634</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B41">
-        <v>345811.8509762709</v>
+        <v>345811.85097627091</v>
       </c>
       <c r="C41">
-        <v>-1694478.069783727</v>
+        <v>-1694478.0697837269</v>
       </c>
       <c r="D41">
-        <v>-0.01486062755769848</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
+        <v>-1.4860627557698481E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B42">
-        <v>301871.7843221913</v>
+        <v>301871.78432219132</v>
       </c>
       <c r="C42">
-        <v>-452807.676483287</v>
+        <v>-452807.67648328701</v>
       </c>
       <c r="D42">
-        <v>-0.003971137989613406</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+        <v>-3.9711379896134064E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>34</v>
       </c>
@@ -1171,27 +1227,27 @@
         <v>127963.0998558381</v>
       </c>
       <c r="C43">
-        <v>-691000.7392215255</v>
+        <v>-691000.73922152549</v>
       </c>
       <c r="D43">
-        <v>-0.006060098865119015</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+        <v>-6.0600988651190154E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B44">
-        <v>213694.1023588947</v>
+        <v>213694.10235889471</v>
       </c>
       <c r="C44">
         <v>-1047101.101558584</v>
       </c>
       <c r="D44">
-        <v>-0.009183110577231602</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>-9.1831105772316023E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>15</v>
       </c>
@@ -1202,7 +1258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>36</v>
       </c>
@@ -1216,7 +1272,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>37</v>
       </c>
@@ -1230,7 +1286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>15</v>
       </c>
@@ -1243,16 +1299,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A31:A32"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A13"/>
     <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A31:A32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add bwaise benchmark and comparison
</commit_message>
<xml_diff>
--- a/exposan/bwaise/results/sysA_lca.xlsx
+++ b/exposan/bwaise/results/sysA_lca.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10912"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfca01abaf64aab7/Coding/es/exposan/bwaise/results/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_AF7EC334C04848CC09694F1B952C58BD60B4E223" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{308E5445-4921-9A4A-AD00-B9F817516E7B}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="23380" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="LCA" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -94,7 +88,7 @@
     <t>Transportation</t>
   </si>
   <si>
-    <t>item26 [tonne*km]</t>
+    <t>item32 [tonne*km]</t>
   </si>
   <si>
     <t>A3</t>
@@ -139,8 +133,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,11 +186,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -206,14 +197,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -260,7 +243,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -292,27 +275,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -344,24 +309,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -537,17 +484,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -567,46 +511,46 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C2">
-        <v>6473254.7249999996</v>
+        <v>6473254.725</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
-        <v>1812511.3230000001</v>
+        <v>1812511.323</v>
       </c>
       <c r="F2">
-        <v>5.7843849083215548E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
+        <v>0.05786408389956039</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C3">
-        <v>6473254.7249999996</v>
+        <v>6473254.725</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>1812511.3230000001</v>
+        <v>1812511.323</v>
       </c>
       <c r="F3">
-        <v>5.7843849083215548E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+        <v>0.05786408389956039</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -622,11 +566,11 @@
         <v>21577515.75</v>
       </c>
       <c r="F4">
-        <v>0.68861725099066129</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
+        <v>0.6888581416614331</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
@@ -640,11 +584,11 @@
         <v>21577515.75</v>
       </c>
       <c r="F5">
-        <v>0.68861725099066129</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+        <v>0.6888581416614331</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -654,149 +598,149 @@
         <v>433.0444991846079</v>
       </c>
       <c r="D6">
-        <v>6.671270848009403E-2</v>
+        <v>0.06671270848009403</v>
       </c>
       <c r="E6">
         <v>129913.3497553824</v>
       </c>
       <c r="F6">
-        <v>4.1460089665576868E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
+        <v>0.004147459314889134</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C7">
-        <v>6058.1399999999994</v>
+        <v>6058.139999999999</v>
       </c>
       <c r="D7">
-        <v>0.93328729151990597</v>
+        <v>0.933287291519906</v>
       </c>
       <c r="E7">
         <v>1817442</v>
       </c>
       <c r="F7">
-        <v>5.800120497536744E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
+        <v>0.05802149483762691</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C8">
-        <v>6491.1844991846074</v>
+        <v>6491.184499184607</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8">
-        <v>1947355.3497553819</v>
+        <v>1947355.349755382</v>
       </c>
       <c r="F8">
-        <v>6.2147213941925128E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+        <v>0.06216895415251604</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C9">
-        <v>104348.40949999999</v>
+        <v>104348.4095</v>
       </c>
       <c r="D9">
-        <v>0.73083545538470884</v>
+        <v>0.7383399407746113</v>
       </c>
       <c r="E9">
-        <v>55304.657035000018</v>
+        <v>55304.65703500002</v>
       </c>
       <c r="F9">
-        <v>1.7649733794968051E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
+        <v>0.001765590798855193</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C10">
-        <v>1451.211728244062</v>
+        <v>13920</v>
       </c>
       <c r="D10">
-        <v>1.0163997605261821E-2</v>
+        <v>0.09849399741528966</v>
       </c>
       <c r="E10">
-        <v>769.14221596935306</v>
+        <v>7377.6</v>
       </c>
       <c r="F10">
-        <v>2.4546134250032069E-5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
+        <v>0.0002355284957176495</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C11">
-        <v>13920</v>
+        <v>23060</v>
       </c>
       <c r="D11">
-        <v>9.7492904661427973E-2</v>
+        <v>0.1631660618100991</v>
       </c>
       <c r="E11">
-        <v>7377.6</v>
+        <v>12221.8</v>
       </c>
       <c r="F11">
-        <v>2.354461324357371E-4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
+        <v>0.0003901786717851291</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C12">
-        <v>23060</v>
+        <v>141328.4095</v>
       </c>
       <c r="D12">
-        <v>0.16150764234860121</v>
+        <v>1</v>
       </c>
       <c r="E12">
-        <v>12221.8</v>
+        <v>74904.05703500001</v>
       </c>
       <c r="F12">
-        <v>3.9004222801494948E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
+        <v>0.002391297966357972</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13">
+        <v>36533360</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>548000.4</v>
+      </c>
+      <c r="F13">
+        <v>0.01749480994695703</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C13">
-        <v>142779.6212282441</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>75673.199250969381</v>
-      </c>
-      <c r="F13">
-        <v>2.415007874197525E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="C14">
         <v>36533360</v>
@@ -808,234 +752,234 @@
         <v>548000.4</v>
       </c>
       <c r="F14">
-        <v>1.7488692088651711E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
+        <v>0.01749480994695703</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15">
+        <v>287700.21</v>
+      </c>
+      <c r="D15">
+        <v>0.9473102251044178</v>
+      </c>
+      <c r="E15">
+        <v>566769.4137</v>
+      </c>
+      <c r="F15">
+        <v>0.01809400718764031</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <v>4539.973846153845</v>
+      </c>
+      <c r="D16">
+        <v>0.01494876783777171</v>
+      </c>
+      <c r="E16">
+        <v>8943.748476923076</v>
+      </c>
+      <c r="F16">
+        <v>0.0002855274919820417</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>11462.02729411765</v>
+      </c>
+      <c r="D17">
+        <v>0.03774100705781051</v>
+      </c>
+      <c r="E17">
+        <v>22580.19376941176</v>
+      </c>
+      <c r="F17">
+        <v>0.0007208684492955153</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C15">
-        <v>36533360</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>548000.4</v>
-      </c>
-      <c r="F15">
-        <v>1.7488692088651711E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="1" t="s">
+      <c r="C18">
+        <v>303702.2111402715</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>598293.3559463349</v>
+      </c>
+      <c r="F18">
+        <v>0.01910040312891787</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C16">
-        <v>287700.21000000002</v>
-      </c>
-      <c r="D16">
-        <v>0.94731022510441776</v>
-      </c>
-      <c r="E16">
-        <v>566769.41370000003</v>
-      </c>
-      <c r="F16">
-        <v>1.8087679792688039E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
-      <c r="B17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17">
-        <v>4539.9738461538454</v>
-      </c>
-      <c r="D17">
-        <v>1.494876783777171E-2</v>
-      </c>
-      <c r="E17">
-        <v>8943.7484769230759</v>
-      </c>
-      <c r="F17">
-        <v>2.8542764427043381E-4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
-      <c r="B18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18">
-        <v>11462.02729411765</v>
-      </c>
-      <c r="D18">
-        <v>3.7741007057810513E-2</v>
-      </c>
-      <c r="E18">
-        <v>22580.193769411759</v>
-      </c>
-      <c r="F18">
-        <v>7.2061636476056267E-4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
-      <c r="B19" s="1" t="s">
+      <c r="C19">
+        <v>90545649.425</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1086547.7931</v>
+      </c>
+      <c r="F19">
+        <v>0.03468783442232905</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C19">
-        <v>303702.21114027151</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>598293.35594633489</v>
-      </c>
-      <c r="F19">
-        <v>1.9093723801719031E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20">
+        <v>90545649.425</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1086547.7931</v>
+      </c>
+      <c r="F20">
+        <v>0.03468783442232905</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C20">
-        <v>90545649.424999997</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>1086547.7930999999</v>
-      </c>
-      <c r="F20">
-        <v>3.4675704238774183E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
-      <c r="B21" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="C21">
-        <v>90545649.424999997</v>
+        <v>958287.1578125</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0.9290978436585084</v>
       </c>
       <c r="E21">
-        <v>1086547.7930999999</v>
+        <v>2443632.252421875</v>
       </c>
       <c r="F21">
-        <v>3.4675704238774183E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>13</v>
-      </c>
+        <v>0.07801250115214375</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C22">
-        <v>958287.15781250002</v>
+        <v>3831.198962564325</v>
       </c>
       <c r="D22">
-        <v>0.9325618456531295</v>
+        <v>0.003714501092627287</v>
       </c>
       <c r="E22">
-        <v>2443632.252421875</v>
+        <v>9769.557354539027</v>
       </c>
       <c r="F22">
-        <v>7.7985220522657675E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
+        <v>0.0003118912854508073</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C23">
-        <v>69298.478764078478</v>
+        <v>69298.47876407848</v>
       </c>
       <c r="D23">
-        <v>6.7438154346870505E-2</v>
+        <v>0.06718765524886428</v>
       </c>
       <c r="E23">
-        <v>176711.12084840011</v>
+        <v>176711.1208484001</v>
       </c>
       <c r="F23">
-        <v>5.6394965791232857E-3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="2"/>
+        <v>0.005641469376220376</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C24">
-        <v>1027585.636576578</v>
+        <v>1031416.835539143</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24">
-        <v>2620343.3732702751</v>
+        <v>2630112.930624814</v>
       </c>
       <c r="F24">
-        <v>8.362471710178096E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+        <v>0.08396586181381493</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C25">
-        <v>5422.9206249999997</v>
+        <v>5422.920625</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25">
-        <v>1068315.3631249999</v>
+        <v>1068315.363125</v>
       </c>
       <c r="F25">
-        <v>3.4093840879074667E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="2"/>
+        <v>0.03410576751638551</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C26">
-        <v>5422.9206249999997</v>
+        <v>5422.920625</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26">
-        <v>1068315.3631249999</v>
+        <v>1068315.363125</v>
       </c>
       <c r="F26">
-        <v>3.4093840879074667E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.03410576751638551</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
         <v>15</v>
       </c>
@@ -1043,13 +987,13 @@
         <v>22</v>
       </c>
       <c r="E27">
-        <v>31334555.90744796</v>
+        <v>31323598.35068209</v>
       </c>
       <c r="F27">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
         <v>23</v>
       </c>
@@ -1069,45 +1013,45 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+    <row r="31" spans="1:6">
+      <c r="A31" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C31">
-        <v>4932003.6000000034</v>
+        <v>4932003.600000003</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31">
-        <v>956808.69840000069</v>
+        <v>956808.6984000007</v>
       </c>
       <c r="F31">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="2"/>
+    <row r="32" spans="1:6">
+      <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C32">
-        <v>4932003.6000000034</v>
+        <v>4932003.600000003</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32">
-        <v>956808.69840000069</v>
+        <v>956808.6984000007</v>
       </c>
       <c r="F32">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6">
       <c r="A33" s="1" t="s">
         <v>15</v>
       </c>
@@ -1115,13 +1059,13 @@
         <v>22</v>
       </c>
       <c r="E33">
-        <v>956808.69840000069</v>
+        <v>956808.6984000007</v>
       </c>
       <c r="F33">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6">
       <c r="A36" s="1" t="s">
         <v>27</v>
       </c>
@@ -1135,35 +1079,35 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6">
       <c r="A37" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B37">
-        <v>4911701.1664478192</v>
+        <v>6257092.924084017</v>
       </c>
       <c r="C37">
-        <v>137527632.66053891</v>
+        <v>175198601.8743525</v>
       </c>
       <c r="D37">
-        <v>1.206121793078792</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.9597630246013352</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B38">
-        <v>2982.0832979280131</v>
+        <v>67739.48234981557</v>
       </c>
       <c r="C38">
-        <v>790252.07395092328</v>
+        <v>17950962.82270113</v>
       </c>
       <c r="D38">
-        <v>6.9305362855373847E-3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.09833794441794504</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" s="1" t="s">
         <v>30</v>
       </c>
@@ -1171,94 +1115,94 @@
         <v>1979814.487023849</v>
       </c>
       <c r="C39">
-        <v>-2969721.7305357731</v>
+        <v>-2969721.730535773</v>
       </c>
       <c r="D39">
-        <v>-2.6044555768803001E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-0.01626856082086448</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B40">
-        <v>3229279.821138782</v>
+        <v>775639.7358303178</v>
       </c>
       <c r="C40">
-        <v>-17438111.034149431</v>
+        <v>-4188454.573483717</v>
       </c>
       <c r="D40">
-        <v>-0.1529327986058634</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-0.02294495382294777</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B41">
-        <v>345811.85097627091</v>
+        <v>345811.8509762709</v>
       </c>
       <c r="C41">
-        <v>-1694478.0697837269</v>
+        <v>-1694478.069783727</v>
       </c>
       <c r="D41">
-        <v>-1.4860627557698481E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-0.009282593468083709</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B42">
-        <v>301871.78432219132</v>
+        <v>301871.7843221913</v>
       </c>
       <c r="C42">
-        <v>-452807.67648328701</v>
+        <v>-452807.676483287</v>
       </c>
       <c r="D42">
-        <v>-3.9711379896134064E-3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-0.002480545281154566</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B43">
-        <v>127963.0998558381</v>
+        <v>46925.39846119798</v>
       </c>
       <c r="C43">
-        <v>-691000.73922152549</v>
+        <v>-253397.1516904691</v>
       </c>
       <c r="D43">
-        <v>-6.0600988651190154E-3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-0.001388145876336531</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B44">
-        <v>213694.10235889471</v>
+        <v>213694.1023588947</v>
       </c>
       <c r="C44">
         <v>-1047101.101558584</v>
       </c>
       <c r="D44">
-        <v>-9.1831105772316023E-3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-0.005736169749893279</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C45">
-        <v>114024664.3827575</v>
+        <v>182543604.3935181</v>
       </c>
       <c r="D45">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6">
       <c r="A48" s="1" t="s">
         <v>36</v>
       </c>
@@ -1272,7 +1216,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4">
       <c r="A49" s="1" t="s">
         <v>37</v>
       </c>
@@ -1280,18 +1224,18 @@
         <v>456960</v>
       </c>
       <c r="C49">
-        <v>68544</v>
+        <v>51864.96</v>
       </c>
       <c r="D49">
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4">
       <c r="A50" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C50">
-        <v>68544</v>
+        <v>51864.96</v>
       </c>
       <c r="D50">
         <v>1</v>
@@ -1299,16 +1243,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A31:A32"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A9:A13"/>
-    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A31:A32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>